<commit_message>
Documentacion Testing - registrarApicultor
</commit_message>
<xml_diff>
--- a/Documentacion/Documentacion Testing.xlsx
+++ b/Documentacion/Documentacion Testing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>Operación</t>
   </si>
@@ -49,6 +49,93 @@
   </si>
   <si>
     <t>ejemplo</t>
+  </si>
+  <si>
+    <t>inicializarSistema</t>
+  </si>
+  <si>
+    <t>Inicializar sistema con una cantidad de puntos erronea</t>
+  </si>
+  <si>
+    <t>cantPuntos=0</t>
+  </si>
+  <si>
+    <t>Inicializar sistema con una cantidad de puntos valida</t>
+  </si>
+  <si>
+    <t>cantPuntos=3</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>destruirSistema</t>
+  </si>
+  <si>
+    <t>Eliminar el sistema y sus estructuras. Se inicializo el sistema previamente con cantPuntos=3</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Registrar apicultor con formato de cedula invalido</t>
+  </si>
+  <si>
+    <t>TipoRetorno dominio.Sistema.registrarApicultor(String cedula, String nombre, String dirección, String email, String celular)</t>
+  </si>
+  <si>
+    <t>ERROR_1</t>
+  </si>
+  <si>
+    <t>Registrar apicultor con numero de celular invalido</t>
+  </si>
+  <si>
+    <t>ERROR_2</t>
+  </si>
+  <si>
+    <t>Registrar apicultor con email invalido</t>
+  </si>
+  <si>
+    <t>ERROR_3</t>
+  </si>
+  <si>
+    <t>Inicializar sistema despues de destruir una instancia del mismo.</t>
+  </si>
+  <si>
+    <t>3.468.908-7, unNombre, dir, email@mail.com, 901231456</t>
+  </si>
+  <si>
+    <t>ERROR_4</t>
+  </si>
+  <si>
+    <t>Registrar apicultor correctamente.</t>
+  </si>
+  <si>
+    <t>5.468.208-6, unNombre, dir, algo.com, 09978934</t>
+  </si>
+  <si>
+    <t>1.468.902-6, unNombre, dir, email@mail.com, 09978934</t>
+  </si>
+  <si>
+    <t>1.334.908-6, Mario, R. 11, email@mail.com, 099789341</t>
+  </si>
+  <si>
+    <t>3.434.908-6, unNombre, dir, @d.com, 095123412</t>
+  </si>
+  <si>
+    <t>Registrar apicultor duplicado. Ya se ingreso en el sistema un apicultor con cedula 1.334.908-6</t>
+  </si>
+  <si>
+    <t>1.24.567-8, unNombre, dir, email@mail.com, 099927834</t>
+  </si>
+  <si>
+    <t>123.515-7, unNombre, dir, email@mail.com, 097777890</t>
+  </si>
+  <si>
+    <t>1.702.51a-0, unNombre, dir, email@mail.com, 986987</t>
+  </si>
+  <si>
+    <t>567.515--7, unNombre, dir, email@mail.com, 12312</t>
   </si>
 </sst>
 </file>
@@ -98,10 +185,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -114,6 +211,68 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Open Declaration">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1724025" y="0"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F3"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,6 +577,11 @@
     <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -455,9 +619,232 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C18:C19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>